<commit_message>
implement pulp instead od gurobi
</commit_message>
<xml_diff>
--- a/results/emission.xlsx
+++ b/results/emission.xlsx
@@ -479,10 +479,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-9.681400992639004</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-9.681400992639004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -499,10 +499,10 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>72.37567578953416</v>
+        <v>33.23912340812262</v>
       </c>
       <c r="F3" t="n">
-        <v>72.37567578953416</v>
+        <v>33.23912340812262</v>
       </c>
     </row>
     <row r="4">
@@ -519,10 +519,10 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>41.46099436664432</v>
+        <v>-8.116932572908174</v>
       </c>
       <c r="F4" t="n">
-        <v>41.46099436664432</v>
+        <v>-8.116932572908174</v>
       </c>
     </row>
     <row r="5">
@@ -539,10 +539,10 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>19.04763982330304</v>
+        <v>-18.86411409169933</v>
       </c>
       <c r="F5" t="n">
-        <v>19.04763982330304</v>
+        <v>-18.86411409169933</v>
       </c>
     </row>
     <row r="6">
@@ -559,10 +559,10 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>5.913108116443283</v>
+        <v>-14.2165379802521</v>
       </c>
       <c r="F6" t="n">
-        <v>5.913108116443283</v>
+        <v>-14.2165379802521</v>
       </c>
     </row>
     <row r="7">
@@ -579,10 +579,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.5916352909168173</v>
+        <v>-11.40996652814376</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.5916352909168173</v>
+        <v>-11.40996652814376</v>
       </c>
     </row>
     <row r="8">
@@ -599,10 +599,10 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>-15.76936990809035</v>
+        <v>-16.52778345848755</v>
       </c>
       <c r="F8" t="n">
-        <v>-15.76936990809035</v>
+        <v>-16.52778345848755</v>
       </c>
     </row>
     <row r="9">
@@ -619,10 +619,10 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>-20.72990003274473</v>
+        <v>-16.52778345848755</v>
       </c>
       <c r="F9" t="n">
-        <v>-20.72990003274473</v>
+        <v>-16.52778345848755</v>
       </c>
     </row>
     <row r="10">
@@ -639,10 +639,10 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>-29.05981141111232</v>
+        <v>-16.52778345848766</v>
       </c>
       <c r="F10" t="n">
-        <v>-29.05981141111232</v>
+        <v>-16.52778345848766</v>
       </c>
     </row>
     <row r="11">
@@ -659,10 +659,10 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>-32.61627617665665</v>
+        <v>-16.52778345848755</v>
       </c>
       <c r="F11" t="n">
-        <v>-32.61627617665665</v>
+        <v>-16.52778345848755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
build min_em obj function
</commit_message>
<xml_diff>
--- a/results/emission.xlsx
+++ b/results/emission.xlsx
@@ -479,10 +479,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>-7.294328428059155</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>-7.294328428059155</v>
       </c>
     </row>
     <row r="3">
@@ -579,10 +579,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>-11.40996652814376</v>
+        <v>-17.13070542992969</v>
       </c>
       <c r="F7" t="n">
-        <v>-11.40996652814376</v>
+        <v>-17.13070542992969</v>
       </c>
     </row>
     <row r="8">
@@ -590,19 +590,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>5.229794157038724</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>5.229794157038724</v>
       </c>
       <c r="E8" t="n">
-        <v>-16.52778345848755</v>
+        <v>33.23912340812262</v>
       </c>
       <c r="F8" t="n">
-        <v>-16.52778345848755</v>
+        <v>38.46891756516135</v>
       </c>
     </row>
     <row r="9">
@@ -610,19 +610,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>4.139652452119747</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>4.139652452119747</v>
       </c>
       <c r="E9" t="n">
-        <v>-16.52778345848755</v>
+        <v>-8.116932572908174</v>
       </c>
       <c r="F9" t="n">
-        <v>-16.52778345848755</v>
+        <v>-3.977280120788428</v>
       </c>
     </row>
     <row r="10">
@@ -630,19 +630,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>3.276748933086955</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>3.276748933086955</v>
       </c>
       <c r="E10" t="n">
-        <v>-16.52778345848766</v>
+        <v>-35.15785750188112</v>
       </c>
       <c r="F10" t="n">
-        <v>-16.52778345848766</v>
+        <v>-31.88110856879416</v>
       </c>
     </row>
     <row r="11">
@@ -650,19 +650,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>4.685633849059211</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>4.685633849059211</v>
       </c>
       <c r="E11" t="n">
-        <v>-16.52778345848755</v>
+        <v>-1.433666666666667</v>
       </c>
       <c r="F11" t="n">
-        <v>-16.52778345848755</v>
+        <v>3.251967182392544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create biodiversity indicatores for age and species
</commit_message>
<xml_diff>
--- a/results/emission.xlsx
+++ b/results/emission.xlsx
@@ -479,10 +479,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-7.294328428059155</v>
+        <v>-2515007.418206576</v>
       </c>
       <c r="F2" t="n">
-        <v>-7.294328428059155</v>
+        <v>-2515007.418206576</v>
       </c>
     </row>
     <row r="3">
@@ -490,19 +490,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>876663.5182445209</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>876663.5182445209</v>
       </c>
       <c r="E3" t="n">
-        <v>33.23912340812262</v>
+        <v>1306319.689602927</v>
       </c>
       <c r="F3" t="n">
-        <v>33.23912340812262</v>
+        <v>2182983.207847448</v>
       </c>
     </row>
     <row r="4">
@@ -510,19 +510,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1165700.198931394</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1165700.198931394</v>
       </c>
       <c r="E4" t="n">
-        <v>-8.116932572908174</v>
+        <v>-401483.2380664512</v>
       </c>
       <c r="F4" t="n">
-        <v>-8.116932572908174</v>
+        <v>764216.9608649432</v>
       </c>
     </row>
     <row r="5">
@@ -530,19 +530,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1390816.352275759</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1390816.352275759</v>
       </c>
       <c r="E5" t="n">
-        <v>-18.86411409169933</v>
+        <v>-1502979.778848212</v>
       </c>
       <c r="F5" t="n">
-        <v>-18.86411409169933</v>
+        <v>-112163.426572453</v>
       </c>
     </row>
     <row r="6">
@@ -550,19 +550,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1453091.396268783</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1453091.396268783</v>
       </c>
       <c r="E6" t="n">
-        <v>-14.2165379802521</v>
+        <v>-1473402.664590993</v>
       </c>
       <c r="F6" t="n">
-        <v>-14.2165379802521</v>
+        <v>-20311.26832220983</v>
       </c>
     </row>
     <row r="7">
@@ -570,19 +570,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1485408.60282823</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1485408.60282823</v>
       </c>
       <c r="E7" t="n">
-        <v>-17.13070542992969</v>
+        <v>-759328.4909590487</v>
       </c>
       <c r="F7" t="n">
-        <v>-17.13070542992969</v>
+        <v>726080.1118691813</v>
       </c>
     </row>
     <row r="8">
@@ -590,19 +590,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>5.229794157038724</v>
+        <v>1417358.485838958</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>5.229794157038724</v>
+        <v>1417358.485838958</v>
       </c>
       <c r="E8" t="n">
-        <v>33.23912340812262</v>
+        <v>-2833412.93896434</v>
       </c>
       <c r="F8" t="n">
-        <v>38.46891756516135</v>
+        <v>-1416054.453125382</v>
       </c>
     </row>
     <row r="9">
@@ -610,19 +610,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>4.139652452119747</v>
+        <v>1486404.488605577</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>4.139652452119747</v>
+        <v>1486404.488605577</v>
       </c>
       <c r="E9" t="n">
-        <v>-8.116932572908174</v>
+        <v>-1444270.181108203</v>
       </c>
       <c r="F9" t="n">
-        <v>-3.977280120788428</v>
+        <v>42134.30749737332</v>
       </c>
     </row>
     <row r="10">
@@ -630,19 +630,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>3.276748933086955</v>
+        <v>1237228.929894109</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>3.276748933086955</v>
+        <v>1237228.929894109</v>
       </c>
       <c r="E10" t="n">
-        <v>-35.15785750188112</v>
+        <v>-3076644.03439256</v>
       </c>
       <c r="F10" t="n">
-        <v>-31.88110856879416</v>
+        <v>-1839415.10449845</v>
       </c>
     </row>
     <row r="11">
@@ -650,19 +650,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>4.685633849059211</v>
+        <v>979493.4069906169</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>4.685633849059211</v>
+        <v>979493.4069906169</v>
       </c>
       <c r="E11" t="n">
-        <v>-1.433666666666667</v>
+        <v>-7738433.732811249</v>
       </c>
       <c r="F11" t="n">
-        <v>3.251967182392544</v>
+        <v>-6758940.325820632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>